<commit_message>
1.computer codes with time.xlsx
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\Misesq\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7275"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -175,13 +170,18 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>2</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>021-03-31 00:00:00</t>
     </r>
@@ -191,35 +191,374 @@
   </si>
   <si>
     <t>2021-09-30 00:00:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-02-07 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -227,9 +566,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -241,17 +822,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,355 +1134,358 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.5727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;P</oddHeader>
-    <oddFooter>&amp;F</oddFooter>
+    <oddHeader>&amp;C&amp;P</oddHeader>
+    <oddFooter>&amp;C&amp;F</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1.oops oops the new MisesqEx.py
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Weaver\Universa\Misesq\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7275"/>
+    <workbookView windowWidth="19200" windowHeight="7270"/>
   </bookViews>
   <sheets>
     <sheet name="analy" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -178,7 +173,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>2</t>
     </r>
@@ -186,7 +181,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>021-03-31 00:00:00</t>
     </r>
@@ -196,13 +191,22 @@
   </si>
   <si>
     <t>2021-09-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-02-07 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -211,23 +215,355 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -235,9 +571,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -250,17 +828,61 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -518,352 +1140,352 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.70909090909091" defaultRowHeight="12.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="2" width="19.5727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
+    <row r="55" spans="1:1">
+      <c r="A55" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>